<commit_message>
Export PAD fitting result
</commit_message>
<xml_diff>
--- a/Notebooks/beta_good1_gauss3.xlsx
+++ b/Notebooks/beta_good1_gauss3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>phase</t>
   </si>
@@ -81,6 +81,54 @@
   </si>
   <si>
     <t>ne_beta1m3</t>
+  </si>
+  <si>
+    <t>he_beta1_opt</t>
+  </si>
+  <si>
+    <t>he_beta2_opt</t>
+  </si>
+  <si>
+    <t>he_beta3_opt</t>
+  </si>
+  <si>
+    <t>he_beta4_opt</t>
+  </si>
+  <si>
+    <t>he_beta1_err</t>
+  </si>
+  <si>
+    <t>he_beta2_err</t>
+  </si>
+  <si>
+    <t>he_beta3_err</t>
+  </si>
+  <si>
+    <t>he_beta4_err</t>
+  </si>
+  <si>
+    <t>ne_beta1_opt</t>
+  </si>
+  <si>
+    <t>ne_beta2_opt</t>
+  </si>
+  <si>
+    <t>ne_beta3_opt</t>
+  </si>
+  <si>
+    <t>ne_beta4_opt</t>
+  </si>
+  <si>
+    <t>ne_beta1_err</t>
+  </si>
+  <si>
+    <t>ne_beta2_err</t>
+  </si>
+  <si>
+    <t>ne_beta3_err</t>
+  </si>
+  <si>
+    <t>ne_beta4_err</t>
   </si>
   <si>
     <t>he_beta1_amp_err</t>
@@ -606,13 +654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:AM12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:39">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -679,8 +727,56 @@
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:39">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -750,8 +846,56 @@
       <c r="W2">
         <v>-0.08758098204119746</v>
       </c>
+      <c r="X2">
+        <v>0.4064183668315585</v>
+      </c>
+      <c r="Y2">
+        <v>1.847871540595965</v>
+      </c>
+      <c r="Z2">
+        <v>0.6933555098677516</v>
+      </c>
+      <c r="AA2">
+        <v>1.217898798079673</v>
+      </c>
+      <c r="AB2">
+        <v>0.02484455762102329</v>
+      </c>
+      <c r="AC2">
+        <v>0.04339918815866517</v>
+      </c>
+      <c r="AD2">
+        <v>0.03472794976167653</v>
+      </c>
+      <c r="AE2">
+        <v>0.04239777478352487</v>
+      </c>
+      <c r="AF2">
+        <v>0.1818722195005076</v>
+      </c>
+      <c r="AG2">
+        <v>0.5830717177166138</v>
+      </c>
+      <c r="AH2">
+        <v>0.4661120320955427</v>
+      </c>
+      <c r="AI2">
+        <v>0.529321125650234</v>
+      </c>
+      <c r="AJ2">
+        <v>0.02929886724540455</v>
+      </c>
+      <c r="AK2">
+        <v>0.03995892766672736</v>
+      </c>
+      <c r="AL2">
+        <v>0.04092908062654535</v>
+      </c>
+      <c r="AM2">
+        <v>0.04676140889663472</v>
+      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:39">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -821,8 +965,56 @@
       <c r="W3">
         <v>0.2187017704838112</v>
       </c>
+      <c r="X3">
+        <v>0.04866013591835306</v>
+      </c>
+      <c r="Y3">
+        <v>1.848192186651291</v>
+      </c>
+      <c r="Z3">
+        <v>0.08023436581208197</v>
+      </c>
+      <c r="AA3">
+        <v>1.159263221480175</v>
+      </c>
+      <c r="AB3">
+        <v>0.02083829233649789</v>
+      </c>
+      <c r="AC3">
+        <v>0.03771996880529965</v>
+      </c>
+      <c r="AD3">
+        <v>0.02859670138581951</v>
+      </c>
+      <c r="AE3">
+        <v>0.03647335009360102</v>
+      </c>
+      <c r="AF3">
+        <v>-0.01935637752526267</v>
+      </c>
+      <c r="AG3">
+        <v>0.6405848065118078</v>
+      </c>
+      <c r="AH3">
+        <v>0.1002392498584398</v>
+      </c>
+      <c r="AI3">
+        <v>0.55079164869236</v>
+      </c>
+      <c r="AJ3">
+        <v>0.03256623811472293</v>
+      </c>
+      <c r="AK3">
+        <v>0.0451184137288674</v>
+      </c>
+      <c r="AL3">
+        <v>0.04473065163730416</v>
+      </c>
+      <c r="AM3">
+        <v>0.05246554345918293</v>
+      </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:39">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -892,8 +1084,56 @@
       <c r="W4">
         <v>0.4862325283151649</v>
       </c>
+      <c r="X4">
+        <v>-0.4564801193149743</v>
+      </c>
+      <c r="Y4">
+        <v>1.921124057692779</v>
+      </c>
+      <c r="Z4">
+        <v>-0.6811092736337669</v>
+      </c>
+      <c r="AA4">
+        <v>1.268420666147432</v>
+      </c>
+      <c r="AB4">
+        <v>0.02240014738461018</v>
+      </c>
+      <c r="AC4">
+        <v>0.03950996720593142</v>
+      </c>
+      <c r="AD4">
+        <v>0.03097381324252533</v>
+      </c>
+      <c r="AE4">
+        <v>0.03822582265117613</v>
+      </c>
+      <c r="AF4">
+        <v>-0.2976304747383203</v>
+      </c>
+      <c r="AG4">
+        <v>0.6752453839146996</v>
+      </c>
+      <c r="AH4">
+        <v>-0.2298204089472384</v>
+      </c>
+      <c r="AI4">
+        <v>0.6307990427884672</v>
+      </c>
+      <c r="AJ4">
+        <v>0.03854087460589876</v>
+      </c>
+      <c r="AK4">
+        <v>0.05264180297992035</v>
+      </c>
+      <c r="AL4">
+        <v>0.05217664245567467</v>
+      </c>
+      <c r="AM4">
+        <v>0.06138732717558313</v>
+      </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:39">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -963,8 +1203,56 @@
       <c r="W5">
         <v>0.2062015503657257</v>
       </c>
+      <c r="X5">
+        <v>-0.7102288879290288</v>
+      </c>
+      <c r="Y5">
+        <v>1.919533556283011</v>
+      </c>
+      <c r="Z5">
+        <v>-0.9457262842406051</v>
+      </c>
+      <c r="AA5">
+        <v>1.348834407013513</v>
+      </c>
+      <c r="AB5">
+        <v>0.03044626199426821</v>
+      </c>
+      <c r="AC5">
+        <v>0.05066757928965154</v>
+      </c>
+      <c r="AD5">
+        <v>0.04154600255670721</v>
+      </c>
+      <c r="AE5">
+        <v>0.04976826915490146</v>
+      </c>
+      <c r="AF5">
+        <v>-0.4934122918355285</v>
+      </c>
+      <c r="AG5">
+        <v>0.603834761065284</v>
+      </c>
+      <c r="AH5">
+        <v>-0.2327297784336328</v>
+      </c>
+      <c r="AI5">
+        <v>0.5884053722012025</v>
+      </c>
+      <c r="AJ5">
+        <v>0.03252723123382015</v>
+      </c>
+      <c r="AK5">
+        <v>0.04254193123138601</v>
+      </c>
+      <c r="AL5">
+        <v>0.04262932348261868</v>
+      </c>
+      <c r="AM5">
+        <v>0.04992383062896493</v>
+      </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:39">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1034,8 +1322,56 @@
       <c r="W6">
         <v>-0.05643515385717446</v>
       </c>
+      <c r="X6">
+        <v>-0.4559414939005225</v>
+      </c>
+      <c r="Y6">
+        <v>1.847661548368638</v>
+      </c>
+      <c r="Z6">
+        <v>-0.4823342111185661</v>
+      </c>
+      <c r="AA6">
+        <v>1.294343388109148</v>
+      </c>
+      <c r="AB6">
+        <v>0.02977461049766058</v>
+      </c>
+      <c r="AC6">
+        <v>0.05154688892186666</v>
+      </c>
+      <c r="AD6">
+        <v>0.04013189115553188</v>
+      </c>
+      <c r="AE6">
+        <v>0.05105467125719609</v>
+      </c>
+      <c r="AF6">
+        <v>-0.4006310079595611</v>
+      </c>
+      <c r="AG6">
+        <v>0.5906102365503573</v>
+      </c>
+      <c r="AH6">
+        <v>0.1121240532922633</v>
+      </c>
+      <c r="AI6">
+        <v>0.4817147287771337</v>
+      </c>
+      <c r="AJ6">
+        <v>0.05118317527734145</v>
+      </c>
+      <c r="AK6">
+        <v>0.06797494041502988</v>
+      </c>
+      <c r="AL6">
+        <v>0.06790547194782606</v>
+      </c>
+      <c r="AM6">
+        <v>0.07912705115083606</v>
+      </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:39">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1105,8 +1441,56 @@
       <c r="W7">
         <v>-0.3507864007898438</v>
       </c>
+      <c r="X7">
+        <v>0.1247472615625913</v>
+      </c>
+      <c r="Y7">
+        <v>1.807202622383271</v>
+      </c>
+      <c r="Z7">
+        <v>0.4807508293496556</v>
+      </c>
+      <c r="AA7">
+        <v>1.210353099919344</v>
+      </c>
+      <c r="AB7">
+        <v>0.02042460126273658</v>
+      </c>
+      <c r="AC7">
+        <v>0.03647830184288441</v>
+      </c>
+      <c r="AD7">
+        <v>0.02868958204368</v>
+      </c>
+      <c r="AE7">
+        <v>0.03596011615568327</v>
+      </c>
+      <c r="AF7">
+        <v>-0.05571290669522796</v>
+      </c>
+      <c r="AG7">
+        <v>0.5994575865689268</v>
+      </c>
+      <c r="AH7">
+        <v>0.5419226240470545</v>
+      </c>
+      <c r="AI7">
+        <v>0.5226682230183728</v>
+      </c>
+      <c r="AJ7">
+        <v>0.03363369274964349</v>
+      </c>
+      <c r="AK7">
+        <v>0.04628774258723273</v>
+      </c>
+      <c r="AL7">
+        <v>0.04771303504203463</v>
+      </c>
+      <c r="AM7">
+        <v>0.05400912257121853</v>
+      </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:39">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1176,8 +1560,56 @@
       <c r="W8">
         <v>-0.3256822438487434</v>
       </c>
+      <c r="X8">
+        <v>0.4318461611565374</v>
+      </c>
+      <c r="Y8">
+        <v>1.815726743899061</v>
+      </c>
+      <c r="Z8">
+        <v>0.7988007946000484</v>
+      </c>
+      <c r="AA8">
+        <v>1.156683545777771</v>
+      </c>
+      <c r="AB8">
+        <v>0.02778369108294252</v>
+      </c>
+      <c r="AC8">
+        <v>0.04792272049792755</v>
+      </c>
+      <c r="AD8">
+        <v>0.0393132751000774</v>
+      </c>
+      <c r="AE8">
+        <v>0.04670335206882592</v>
+      </c>
+      <c r="AF8">
+        <v>0.1289084504849409</v>
+      </c>
+      <c r="AG8">
+        <v>0.6146813279844398</v>
+      </c>
+      <c r="AH8">
+        <v>0.5685002418873213</v>
+      </c>
+      <c r="AI8">
+        <v>0.5218260060347322</v>
+      </c>
+      <c r="AJ8">
+        <v>0.03290129914675804</v>
+      </c>
+      <c r="AK8">
+        <v>0.04524159937049346</v>
+      </c>
+      <c r="AL8">
+        <v>0.04668612680857368</v>
+      </c>
+      <c r="AM8">
+        <v>0.05266837024446444</v>
+      </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:39">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1247,8 +1679,56 @@
       <c r="W9">
         <v>0.08087712190525712</v>
       </c>
+      <c r="X9">
+        <v>0.2759798184783597</v>
+      </c>
+      <c r="Y9">
+        <v>1.840859598779039</v>
+      </c>
+      <c r="Z9">
+        <v>0.3962568280452447</v>
+      </c>
+      <c r="AA9">
+        <v>1.042536425716255</v>
+      </c>
+      <c r="AB9">
+        <v>0.02893826558193782</v>
+      </c>
+      <c r="AC9">
+        <v>0.05143308802082835</v>
+      </c>
+      <c r="AD9">
+        <v>0.03976590869248701</v>
+      </c>
+      <c r="AE9">
+        <v>0.04887224369702132</v>
+      </c>
+      <c r="AF9">
+        <v>0.1088402768642438</v>
+      </c>
+      <c r="AG9">
+        <v>0.6809822615139649</v>
+      </c>
+      <c r="AH9">
+        <v>0.3936650274633626</v>
+      </c>
+      <c r="AI9">
+        <v>0.474715666627994</v>
+      </c>
+      <c r="AJ9">
+        <v>0.03502100319546256</v>
+      </c>
+      <c r="AK9">
+        <v>0.04869750334866401</v>
+      </c>
+      <c r="AL9">
+        <v>0.04880478796269962</v>
+      </c>
+      <c r="AM9">
+        <v>0.05589034315231432</v>
+      </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:39">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1318,8 +1798,56 @@
       <c r="W10">
         <v>0.3839470497762129</v>
       </c>
+      <c r="X10">
+        <v>-0.2668050390973027</v>
+      </c>
+      <c r="Y10">
+        <v>1.893066694062168</v>
+      </c>
+      <c r="Z10">
+        <v>-0.3641224808732362</v>
+      </c>
+      <c r="AA10">
+        <v>1.005364398905386</v>
+      </c>
+      <c r="AB10">
+        <v>0.02301321083644349</v>
+      </c>
+      <c r="AC10">
+        <v>0.04149599731777368</v>
+      </c>
+      <c r="AD10">
+        <v>0.0315686808314583</v>
+      </c>
+      <c r="AE10">
+        <v>0.03868031164824302</v>
+      </c>
+      <c r="AF10">
+        <v>-0.1622021102372048</v>
+      </c>
+      <c r="AG10">
+        <v>0.6917725598888117</v>
+      </c>
+      <c r="AH10">
+        <v>-0.03082549158118449</v>
+      </c>
+      <c r="AI10">
+        <v>0.5219086515860299</v>
+      </c>
+      <c r="AJ10">
+        <v>0.03565302840181763</v>
+      </c>
+      <c r="AK10">
+        <v>0.04950086786485219</v>
+      </c>
+      <c r="AL10">
+        <v>0.04863244197139843</v>
+      </c>
+      <c r="AM10">
+        <v>0.05694991999619248</v>
+      </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:39">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1389,8 +1917,56 @@
       <c r="W11">
         <v>0.4604258058666044</v>
       </c>
+      <c r="X11">
+        <v>-0.6253846242292707</v>
+      </c>
+      <c r="Y11">
+        <v>1.875950470638957</v>
+      </c>
+      <c r="Z11">
+        <v>-0.8291200870381218</v>
+      </c>
+      <c r="AA11">
+        <v>1.108339440768152</v>
+      </c>
+      <c r="AB11">
+        <v>0.02032737926003229</v>
+      </c>
+      <c r="AC11">
+        <v>0.03417487227937894</v>
+      </c>
+      <c r="AD11">
+        <v>0.02774968669456299</v>
+      </c>
+      <c r="AE11">
+        <v>0.03253141934791746</v>
+      </c>
+      <c r="AF11">
+        <v>-0.3931675270957805</v>
+      </c>
+      <c r="AG11">
+        <v>0.6619664397733006</v>
+      </c>
+      <c r="AH11">
+        <v>-0.255667623735069</v>
+      </c>
+      <c r="AI11">
+        <v>0.4970636003621927</v>
+      </c>
+      <c r="AJ11">
+        <v>0.03153292051154979</v>
+      </c>
+      <c r="AK11">
+        <v>0.0423763556186801</v>
+      </c>
+      <c r="AL11">
+        <v>0.04215181477177497</v>
+      </c>
+      <c r="AM11">
+        <v>0.04887431484711173</v>
+      </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:39">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1459,6 +2035,54 @@
       </c>
       <c r="W12">
         <v>0.211955776937046</v>
+      </c>
+      <c r="X12">
+        <v>-0.6366319521941426</v>
+      </c>
+      <c r="Y12">
+        <v>1.909210604420869</v>
+      </c>
+      <c r="Z12">
+        <v>-0.7073660454160748</v>
+      </c>
+      <c r="AA12">
+        <v>1.261791614540597</v>
+      </c>
+      <c r="AB12">
+        <v>0.0264311852433526</v>
+      </c>
+      <c r="AC12">
+        <v>0.04469386101317384</v>
+      </c>
+      <c r="AD12">
+        <v>0.03528279963478757</v>
+      </c>
+      <c r="AE12">
+        <v>0.04332130251061016</v>
+      </c>
+      <c r="AF12">
+        <v>-0.4446144601439269</v>
+      </c>
+      <c r="AG12">
+        <v>0.6330034678361081</v>
+      </c>
+      <c r="AH12">
+        <v>-0.115172606613563</v>
+      </c>
+      <c r="AI12">
+        <v>0.4428544523798389</v>
+      </c>
+      <c r="AJ12">
+        <v>0.04244161552391883</v>
+      </c>
+      <c r="AK12">
+        <v>0.05627451251512069</v>
+      </c>
+      <c r="AL12">
+        <v>0.05587603067227861</v>
+      </c>
+      <c r="AM12">
+        <v>0.06489748307809728</v>
       </c>
     </row>
   </sheetData>
@@ -1476,172 +2100,172 @@
   <sheetData>
     <row r="1" spans="1:57">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>55</v>
+        <v>71</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="BA1" s="1" t="s">
-        <v>73</v>
+        <v>89</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="BD1" s="1" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="BE1" s="1" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:57">

</xml_diff>